<commit_message>
TC, G, O, R categories stable
</commit_message>
<xml_diff>
--- a/Belegung_TennishalleDietlikon.xlsx
+++ b/Belegung_TennishalleDietlikon.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F097DB-D9C8-4885-B84C-9754FFFC1096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B211E0A-265C-4624-9035-A40C008052F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{8A5DF991-B628-454A-BE30-B3EC96302676}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,6 +419,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,30 +462,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,7 +781,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,26 +795,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -824,26 +824,26 @@
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17">
+      <c r="A2" s="25">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26">
         <v>6</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26">
         <v>21</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18">
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26">
         <v>5</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="21"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -874,61 +874,61 @@
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="26" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="26" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="26" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="29"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22">
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="19">
         <v>2</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="22">
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="19">
         <v>3</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="22">
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="19">
         <v>4</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22">
+      <c r="L5" s="20"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="19">
         <v>5</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="25"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -1518,16 +1518,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D1:F1"/>
@@ -1536,6 +1526,16 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Stable before updating initial placement strategy
</commit_message>
<xml_diff>
--- a/Belegung_TennishalleDietlikon.xlsx
+++ b/Belegung_TennishalleDietlikon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B211E0A-265C-4624-9035-A40C008052F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB147C09-D2C9-4BAA-935F-983663DC496B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{8A5DF991-B628-454A-BE30-B3EC96302676}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -67,6 +67,9 @@
   <si>
     <t># nDays</t>
   </si>
+  <si>
+    <t>Samstag</t>
+  </si>
 </sst>
 </file>
 
@@ -419,6 +422,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,39 +465,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,7 +784,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,26 +798,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -824,26 +827,26 @@
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25">
+      <c r="A2" s="17">
         <v>3</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18">
         <v>6</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18">
         <v>21</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26">
-        <v>5</v>
-      </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="29"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18">
+        <v>6</v>
+      </c>
+      <c r="K2" s="18"/>
+      <c r="L2" s="21"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -874,61 +877,71 @@
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="15" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="15" t="s">
+      <c r="L4" s="27"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="18"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="27"/>
+      <c r="S4" s="29"/>
     </row>
     <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="19">
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="22">
         <v>2</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="19">
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="22">
         <v>3</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="19">
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="22">
         <v>4</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="19">
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="22">
         <v>5</v>
       </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="22"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="22">
+        <v>6</v>
+      </c>
+      <c r="R5" s="23"/>
+      <c r="S5" s="25"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -958,7 +971,12 @@
         <v>0</v>
       </c>
       <c r="O6" s="6"/>
-      <c r="P6" s="7"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
@@ -988,7 +1006,12 @@
         <v>0</v>
       </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
@@ -1018,7 +1041,12 @@
         <v>0</v>
       </c>
       <c r="O8" s="6"/>
-      <c r="P8" s="7"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="6"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
@@ -1048,7 +1076,12 @@
         <v>0</v>
       </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="7"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="6"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
@@ -1078,7 +1111,12 @@
         <v>0</v>
       </c>
       <c r="O10" s="6"/>
-      <c r="P10" s="7"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="6"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
@@ -1108,7 +1146,12 @@
         <v>0</v>
       </c>
       <c r="O11" s="6"/>
-      <c r="P11" s="7"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="6"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
@@ -1138,7 +1181,12 @@
         <v>0</v>
       </c>
       <c r="O12" s="6"/>
-      <c r="P12" s="7"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="6"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
@@ -1174,9 +1222,12 @@
       <c r="O13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="P13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
@@ -1212,9 +1263,12 @@
       <c r="O14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="P14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
@@ -1250,9 +1304,12 @@
       <c r="O15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="P15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
@@ -1300,11 +1357,14 @@
       <c r="O16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P16" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -1350,11 +1410,14 @@
       <c r="O17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>18</v>
       </c>
@@ -1400,11 +1463,14 @@
       <c r="O18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -1450,11 +1516,14 @@
       <c r="O19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -1492,11 +1561,14 @@
       <c r="O20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P20" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>21</v>
       </c>
@@ -1514,10 +1586,25 @@
       <c r="M21" s="9"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="10"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D1:F1"/>
@@ -1526,16 +1613,6 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
V2 Final - playerUnions
</commit_message>
<xml_diff>
--- a/Belegung_TennishalleDietlikon.xlsx
+++ b/Belegung_TennishalleDietlikon.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB147C09-D2C9-4BAA-935F-983663DC496B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001BA928-404D-45B6-9A7A-16D8203F0E65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{8A5DF991-B628-454A-BE30-B3EC96302676}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -422,6 +423,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,30 +466,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -784,7 +785,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,26 +799,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -827,26 +828,26 @@
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17">
+      <c r="A2" s="25">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26">
         <v>6</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26">
         <v>21</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18">
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26">
         <v>6</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="21"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -877,71 +878,71 @@
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="26" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="26" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="26" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="26" t="s">
+      <c r="O4" s="16"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="29"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="18">
         <v>1</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22">
+      <c r="C5" s="19"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="18">
         <v>2</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="22">
+      <c r="F5" s="19"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="18">
         <v>3</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="22">
+      <c r="I5" s="19"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="18">
         <v>4</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22">
+      <c r="L5" s="19"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="18">
         <v>5</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="22">
+      <c r="O5" s="19"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="18">
         <v>6</v>
       </c>
-      <c r="R5" s="23"/>
-      <c r="S5" s="25"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="20"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -1593,6 +1594,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="Q5:S5"/>
     <mergeCell ref="B4:D4"/>
@@ -1605,16 +1614,22 @@
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N5:P5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F96047-E1E3-4ACE-B5B2-37E2EEA59F46}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:S21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>